<commit_message>
revert changes to facilitate mrege
</commit_message>
<xml_diff>
--- a/standard-observations.xlsx
+++ b/standard-observations.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF95"/>
+  <dimension ref="A1:AF94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2013,27 +2013,111 @@
       <c r="AF35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
-      <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
-      <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Identifier</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>skos:prefLabel@en</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>skos:notation</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>rdf:type(separator=",")</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>skos:definition@en</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>skos:broader(separator=",")</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>dct:source(separator=",")</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>^skos:member</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>skos:exactMatch(separator=",")</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>dct:isReplacedBy</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>skos:closeMatch(separator=",")</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>skos:narrowMatch(separator=",")</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>skos:related(separator=",")</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>obo:RO_0002351(separator=",")</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>skos:broadMatch(separator=",")</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>owl:sameAs(separator=",")</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>rdfs:seeAlso</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>dct:creator</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>dct:contributor</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>dct:created^^xsd:date</t>
+        </is>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>2024-01-05</t>
+        </is>
+      </c>
       <c r="V36" t="inlineStr"/>
       <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr"/>
@@ -2049,107 +2133,59 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t>so:027</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>skos:prefLabel@en</t>
+          <t>Meteorological data</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>skos:notation</t>
+          <t>SOATM_027</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>rdf:type(separator=",")</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>skos:definition@en</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>skos:broader(separator=",")</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>dct:source(separator=",")</t>
-        </is>
-      </c>
+          <t>iop:VariableSet</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>^skos:member</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>skos:exactMatch(separator=",")</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>dct:isReplacedBy</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>skos:closeMatch(separator=",")</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>skos:narrowMatch(separator=",")</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>skos:related(separator=",")</t>
-        </is>
-      </c>
-      <c r="N37" t="inlineStr">
-        <is>
-          <t>obo:RO_0002351(separator=",")</t>
-        </is>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>skos:broadMatch(separator=",")</t>
-        </is>
-      </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>owl:sameAs(separator=",")</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>rdfs:seeAlso</t>
-        </is>
-      </c>
+          <t>so:c5</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr">
         <is>
-          <t>dct:creator</t>
+          <t>http://purl.org/np/RAjk9ru697It_UawXK1gvq-mpaOdGlwyhNb9nF2tfEE2A</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>dct:contributor</t>
+          <t>https://orcid.org/0000-0003-2195-3997</t>
         </is>
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>dct:created^^xsd:date</t>
+          <t>2023-08-16</t>
         </is>
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>2024-01-05</t>
+          <t>2023-09-27</t>
         </is>
       </c>
       <c r="V37" t="inlineStr"/>
@@ -2167,17 +2203,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>so:027</t>
+          <t>so:028</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Meteorological data</t>
+          <t>Radiation</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SOATM_027</t>
+          <t>SOATM_028</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2219,7 +2255,7 @@
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>2023-09-27</t>
+          <t>2023-08-26</t>
         </is>
       </c>
       <c r="V38" t="inlineStr"/>
@@ -2237,17 +2273,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>so:028</t>
+          <t>so:098</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Radiation</t>
+          <t>Ground heat flux</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SOATM_028</t>
+          <t>SOATM_098</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2289,7 +2325,7 @@
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>2023-08-26</t>
+          <t>2023-08-23</t>
         </is>
       </c>
       <c r="V39" t="inlineStr"/>
@@ -2307,17 +2343,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>so:098</t>
+          <t>so:103</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Ground heat flux</t>
+          <t>Atmospheric deposition in precipitation</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SOATM_098</t>
+          <t>SOATM_103</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2377,17 +2413,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>so:103</t>
+          <t>so:108</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Atmospheric deposition in precipitation</t>
+          <t>Dry deposition of N-components</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SOATM_103</t>
+          <t>SOATM_108</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2447,17 +2483,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>so:108</t>
+          <t>so:176</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Dry deposition of N-components</t>
+          <t>CO2 flux and concentration, Latent heat flux, Sensible heat flux - Eddy Covariance</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SOATM_108</t>
+          <t>SOATM_176</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2517,17 +2553,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>so:176</t>
+          <t>so:014</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>CO2 flux and concentration, Latent heat flux, Sensible heat flux - Eddy Covariance</t>
+          <t>Flying insects</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SOATM_176</t>
+          <t>SOBIO_014</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2540,7 +2576,7 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>so:c5</t>
+          <t>so:c4</t>
         </is>
       </c>
       <c r="I43" t="inlineStr"/>
@@ -2587,17 +2623,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>so:014</t>
+          <t>so:015</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Flying insects</t>
+          <t>Vegetation phenology and Leaf Area Index – European scale</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>SOBIO_014</t>
+          <t>SOBIO_015</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2610,7 +2646,7 @@
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>so:c4</t>
+          <t>so:c5</t>
         </is>
       </c>
       <c r="I44" t="inlineStr"/>
@@ -2657,17 +2693,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>so:015</t>
+          <t>so:016</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Vegetation phenology and Leaf Area Index – European scale</t>
+          <t>Vegetation phenology – site scale</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SOBIO_015</t>
+          <t>SOBIO_016</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2727,17 +2763,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>so:016</t>
+          <t>so:017</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Vegetation phenology – site scale</t>
+          <t>Vegetation composition (mainly species level+abundance)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SOBIO_016</t>
+          <t>SOBIO_017</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2750,7 +2786,7 @@
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>so:c5</t>
+          <t>so:c4</t>
         </is>
       </c>
       <c r="I46" t="inlineStr"/>
@@ -2797,17 +2833,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>so:017</t>
+          <t>so:018</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Vegetation composition (mainly species level+abundance)</t>
+          <t>Birds, bats, frogs, insects using acoustic recording</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SOBIO_017</t>
+          <t>SOBIO_018</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2867,17 +2903,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>so:018</t>
+          <t>so:019</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Birds, bats, frogs, insects using acoustic recording</t>
+          <t>Pollen and spores</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SOBIO_018</t>
+          <t>SOBIO_019</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2937,17 +2973,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>so:019</t>
+          <t>so:021</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Pollen and spores</t>
+          <t>eDNA Water</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SOBIO_019</t>
+          <t>SOBIO_021</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3007,17 +3043,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>so:021</t>
+          <t>so:022</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>eDNA Water</t>
+          <t>eDNA soil</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>SOBIO_021</t>
+          <t>SOBIO_022</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -3077,17 +3113,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>so:022</t>
+          <t>so:023</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>eDNA soil</t>
+          <t>Vegetation aboveground biomass - forest (site scale)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SOBIO_022</t>
+          <t>SOBIO_023</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -3100,7 +3136,7 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>so:c4</t>
+          <t>so:c5</t>
         </is>
       </c>
       <c r="I51" t="inlineStr"/>
@@ -3147,17 +3183,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>so:023</t>
+          <t>so:024</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Vegetation aboveground biomass - forest (site scale)</t>
+          <t>Vegetation aboveground biomass – non-forested sites</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SOBIO_023</t>
+          <t>SOBIO_024</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -3217,17 +3253,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>so:024</t>
+          <t>so:025</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Vegetation aboveground biomass – non-forested sites</t>
+          <t>Leaf area index - forests (site scale)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>SOBIO_024</t>
+          <t>SOBIO_025</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -3287,17 +3323,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>so:025</t>
+          <t>so:026</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Leaf area index - forests (site scale)</t>
+          <t>Leaf area index – non-forested sites</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SOBIO_025</t>
+          <t>SOBIO_026</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -3357,17 +3393,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>so:026</t>
+          <t>so:090</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Leaf area index – non-forested sites</t>
+          <t>Gross primary production</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SOBIO_026</t>
+          <t>SOBIO_090</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -3427,17 +3463,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>so:090</t>
+          <t>so:091</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Gross primary production</t>
+          <t>Transpiration (plants)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SOBIO_090</t>
+          <t>SOBIO_091</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -3497,17 +3533,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>so:091</t>
+          <t>so:092</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Transpiration (plants)</t>
+          <t>Aboveground litterfall - forests</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SOBIO_091</t>
+          <t>SOBIO_092</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -3567,17 +3603,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>so:092</t>
+          <t>so:093</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Aboveground litterfall - forests</t>
+          <t>Belowground biomass - terrestrial</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SOBIO_092</t>
+          <t>SOBIO_093</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -3637,17 +3673,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>so:093</t>
+          <t>so:095</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Belowground biomass - terrestrial</t>
+          <t>Leaf C, N, K, P, Ca, Mg, Mn content - terrestrial</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SOBIO_093</t>
+          <t>SOBIO_095</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -3707,17 +3743,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>so:095</t>
+          <t>so:096</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Leaf C, N, K, P, Ca, Mg, Mn content - terrestrial</t>
+          <t>Clorophyll a (benthic, pelagic) - standing, running waters</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SOBIO_095</t>
+          <t>SOBIO_096</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -3730,7 +3766,7 @@
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
         <is>
-          <t>so:c5</t>
+          <t>so:c4</t>
         </is>
       </c>
       <c r="I60" t="inlineStr"/>
@@ -3777,17 +3813,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>so:096</t>
+          <t>so:140</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Clorophyll a (benthic, pelagic) - standing, running waters</t>
+          <t>Vegetation structure - site scale</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SOBIO_096</t>
+          <t>SOBIO_140</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -3800,7 +3836,7 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
         <is>
-          <t>so:c4</t>
+          <t>so:c5</t>
         </is>
       </c>
       <c r="I61" t="inlineStr"/>
@@ -3847,17 +3883,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>so:140</t>
+          <t>so:177</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Vegetation structure - site scale</t>
+          <t>Tree growth</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SOBIO_140</t>
+          <t>SOBIO_177</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -3917,17 +3953,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>so:177</t>
+          <t>so:003</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Tree growth</t>
+          <t>Soil chemical and physical characteristics</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SOBIO_177</t>
+          <t>SOGEO_003</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -3940,7 +3976,7 @@
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr">
         <is>
-          <t>so:c5</t>
+          <t>so:c2</t>
         </is>
       </c>
       <c r="I63" t="inlineStr"/>
@@ -3987,17 +4023,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>so:003</t>
+          <t>so:048</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Soil chemical and physical characteristics</t>
+          <t>Percolation/infiltration - soil</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SOGEO_003</t>
+          <t>SOGEO_048</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -4057,17 +4093,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>so:048</t>
+          <t>so:155</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Percolation/infiltration - soil</t>
+          <t>Sediment (aquatic and marine) inventory</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SOGEO_048</t>
+          <t>SOGEO_155</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -4127,17 +4163,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>so:155</t>
+          <t>so:167</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Sediment (aquatic and marine) inventory</t>
+          <t>Soil water chemical characteristics</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SOGEO_155</t>
+          <t>SOGEO_167</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -4197,17 +4233,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>so:167</t>
+          <t>so:004</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Soil water chemical characteristics</t>
+          <t>Profiles of physical and chemical waters characteristics - surface water (standing)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>SOGEO_167</t>
+          <t>SOHYD_004</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -4220,7 +4256,7 @@
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
         <is>
-          <t>so:c2</t>
+          <t>so:c3</t>
         </is>
       </c>
       <c r="I67" t="inlineStr"/>
@@ -4267,17 +4303,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>so:004</t>
+          <t>so:005</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Profiles of physical and chemical waters characteristics - surface water (standing)</t>
+          <t>Physical and chemical water characteristics - surface water (running waters)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>SOHYD_004</t>
+          <t>SOHYD_005</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -4337,17 +4373,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>so:005</t>
+          <t>so:006</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Physical and chemical water characteristics - surface water (running waters)</t>
+          <t>Physical and chemical water characteristics - groundwater</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SOHYD_005</t>
+          <t>SOHYD_006</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -4407,17 +4443,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>so:006</t>
+          <t>so:010</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Physical and chemical water characteristics - groundwater</t>
+          <t>Water level - surface water (running water)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>SOHYD_006</t>
+          <t>SOHYD_010</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -4477,17 +4513,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>so:010</t>
+          <t>so:011</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Water level - surface water (running water)</t>
+          <t>Ice cover/thickness (standing and transitional water)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SOHYD_010</t>
+          <t>SOHYD_011</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -4547,17 +4583,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>so:011</t>
+          <t>so:012</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Ice cover/thickness (standing and transitional water)</t>
+          <t>Snow cover and depths</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SOHYD_011</t>
+          <t>SOHYD_012</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -4617,17 +4653,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>so:012</t>
+          <t>so:058</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Snow cover and depths</t>
+          <t>Stable isotopes (18O, 2H) - standing, running waters</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SOHYD_012</t>
+          <t>SOHYD_058</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -4687,17 +4723,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>so:058</t>
+          <t>so:059</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Stable isotopes (18O, 2H) - standing, running waters</t>
+          <t>Stable Isotopes (18O, 2H) - groundwater</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>SOHYD_058</t>
+          <t>SOHYD_059</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -4757,17 +4793,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>so:059</t>
+          <t>so:062</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Stable Isotopes (18O, 2H) - groundwater</t>
+          <t>Major ion concentrations: Cl, SO4, Br, Na, K, Mg, Ca, B - groundwater</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>SOHYD_059</t>
+          <t>SOHYD_062</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -4827,17 +4863,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>so:062</t>
+          <t>so:064</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Major ion concentrations: Cl, SO4, Br, Na, K, Mg, Ca, B - groundwater</t>
+          <t>Nutrient concentration: TP, SRP, TDN, NO3, NO2, NH4, DOC, DIC - groundwater</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>SOHYD_062</t>
+          <t>SOHYD_064</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -4897,17 +4933,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>so:064</t>
+          <t>so:065</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Nutrient concentration: TP, SRP, TDN, NO3, NO2, NH4, DOC, DIC - groundwater</t>
+          <t>DOM composition - groundwater</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>SOHYD_064</t>
+          <t>SOHYD_065</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -4967,17 +5003,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>so:065</t>
+          <t>so:067</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>DOM composition - groundwater</t>
+          <t>Micropollutants: non-target screening [~1000 substances] - running waters</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SOHYD_065</t>
+          <t>SOHYD_067</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -5037,17 +5073,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>so:067</t>
+          <t>so:164</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Micropollutants: non-target screening [~1000 substances] - running waters</t>
+          <t>Glacier front variation</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SOHYD_067</t>
+          <t>SOHYD_164</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -5107,17 +5143,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>so:164</t>
+          <t>so:165</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Glacier front variation</t>
+          <t>Glacier mass balance</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SOHYD_164</t>
+          <t>SOHYD_165</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -5177,17 +5213,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>so:165</t>
+          <t>so:166</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Glacier mass balance</t>
+          <t>Glacier area</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>SOHYD_165</t>
+          <t>SOHYD_166</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -5247,17 +5283,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>so:166</t>
+          <t>so:168</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Glacier area</t>
+          <t>Soil water content/soil temperature</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SOHYD_166</t>
+          <t>SOHYD_168</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -5317,17 +5353,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>so:168</t>
+          <t>so:169</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Soil water content/soil temperature</t>
+          <t>Nutrient concentration: NO2, NH4, DOC, DIC - running waters</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>SOHYD_168</t>
+          <t>SOHYD_169</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -5387,17 +5423,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>so:169</t>
+          <t>so:170</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Nutrient concentration: NO2, NH4, DOC, DIC - running waters</t>
+          <t>Profiles of nutrient concentration: NO2, NH4, DOC, DIC - standing waters</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>SOHYD_169</t>
+          <t>SOHYD_170</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -5457,17 +5493,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>so:170</t>
+          <t>so:171</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Profiles of nutrient concentration: NO2, NH4, DOC, DIC - standing waters</t>
+          <t>Major ion concentrations: Cl, SO4, Br, Na, K, Mg, Ca, B, Silica - inland running/standing waters, transitional waters</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>SOHYD_170</t>
+          <t>SOHYD_171</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -5527,17 +5563,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>so:171</t>
+          <t>so:172</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Major ion concentrations: Cl, SO4, Br, Na, K, Mg, Ca, B, Silica - inland running/standing waters, transitional waters</t>
+          <t>Nutrient concentration: TP, SRP, TDN, NO3 - running waters</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>SOHYD_171</t>
+          <t>SOHYD_172</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -5550,7 +5586,7 @@
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr">
         <is>
-          <t>so:c3</t>
+          <t>so:c4</t>
         </is>
       </c>
       <c r="I86" t="inlineStr"/>
@@ -5597,17 +5633,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>so:172</t>
+          <t>so:173</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Nutrient concentration: TP, SRP, TDN, NO3 - running waters</t>
+          <t>Profiles of nutrient concentration: TP, SRP, TDN, NO3, - standing waters</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>SOHYD_172</t>
+          <t>SOHYD_173</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -5667,17 +5703,17 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>so:173</t>
+          <t>so:174</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Profiles of nutrient concentration: TP, SRP, TDN, NO3, - standing waters</t>
+          <t>Secchi-Depth; standing waters and transitional waters</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>SOHYD_173</t>
+          <t>SOHYD_174</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -5690,7 +5726,7 @@
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
         <is>
-          <t>so:c4</t>
+          <t>so:c3</t>
         </is>
       </c>
       <c r="I88" t="inlineStr"/>
@@ -5737,22 +5773,22 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>so:174</t>
+          <t>so:001</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Secchi-Depth; standing waters and transitional waters</t>
+          <t>Soil inventory - pedological/geological characterization</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>SOHYD_174</t>
+          <t>SOGEO_001</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>iop:VariableSet</t>
+          <t>iop:VariableSet,skos:Concept</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
@@ -5760,7 +5796,7 @@
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
         <is>
-          <t>so:c3</t>
+          <t>so:c2</t>
         </is>
       </c>
       <c r="I89" t="inlineStr"/>
@@ -5768,7 +5804,11 @@
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
       <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>et:22245,et:22279,et:30319,et:30321,et:30323,et:30324,et:22065,et:22264,et:30067</t>
+        </is>
+      </c>
       <c r="O89" t="inlineStr"/>
       <c r="P89" t="inlineStr"/>
       <c r="Q89" t="inlineStr"/>
@@ -5789,7 +5829,7 @@
       </c>
       <c r="U89" t="inlineStr">
         <is>
-          <t>2023-08-23</t>
+          <t>2024-01-05</t>
         </is>
       </c>
       <c r="V89" t="inlineStr"/>
@@ -5807,42 +5847,34 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>so:001</t>
+          <t>so:c1</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Soil inventory - pedological/geological characterization</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>SOGEO_001</t>
-        </is>
-      </c>
+          <t>Sociosphere</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr">
         <is>
-          <t>iop:VariableSet</t>
+          <t>skos:Collection</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr"/>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>so:c2</t>
-        </is>
-      </c>
-      <c r="I90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>et:30317</t>
+        </is>
+      </c>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr"/>
       <c r="M90" t="inlineStr"/>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>et:22245,et:22279,et:30319,et:30321,et:30323,et:30324,et:22065,et:22264,et:30067</t>
-        </is>
-      </c>
+      <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
       <c r="P90" t="inlineStr"/>
       <c r="Q90" t="inlineStr"/>
@@ -5863,7 +5895,7 @@
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>2024-01-09</t>
+          <t>2023-08-23</t>
         </is>
       </c>
       <c r="V90" t="inlineStr"/>
@@ -5881,12 +5913,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>so:c1</t>
+          <t>so:c2</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Sociosphere</t>
+          <t>Geosphere</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -5901,7 +5933,7 @@
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr">
         <is>
-          <t>et:30317</t>
+          <t>et:30316</t>
         </is>
       </c>
       <c r="J91" t="inlineStr"/>
@@ -5947,12 +5979,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>so:c2</t>
+          <t>so:c3</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Geosphere</t>
+          <t>Hydrosphere</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -5967,7 +5999,7 @@
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr">
         <is>
-          <t>et:30316</t>
+          <t>et:21922</t>
         </is>
       </c>
       <c r="J92" t="inlineStr"/>
@@ -6013,12 +6045,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>so:c3</t>
+          <t>so:c4</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Hydrosphere</t>
+          <t>Biosphere</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
@@ -6033,7 +6065,7 @@
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr">
         <is>
-          <t>et:21922</t>
+          <t>et:21921</t>
         </is>
       </c>
       <c r="J93" t="inlineStr"/>
@@ -6079,12 +6111,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>so:c4</t>
+          <t>so:c5</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Biosphere</t>
+          <t>Atmosphere</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
@@ -6099,7 +6131,7 @@
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="inlineStr">
         <is>
-          <t>et:21921</t>
+          <t>et:21920</t>
         </is>
       </c>
       <c r="J94" t="inlineStr"/>
@@ -6142,72 +6174,6 @@
       <c r="AE94" t="inlineStr"/>
       <c r="AF94" t="inlineStr"/>
     </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>so:c5</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Atmosphere</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>skos:Collection</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr"/>
-      <c r="H95" t="inlineStr"/>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>et:21920</t>
-        </is>
-      </c>
-      <c r="J95" t="inlineStr"/>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr"/>
-      <c r="N95" t="inlineStr"/>
-      <c r="O95" t="inlineStr"/>
-      <c r="P95" t="inlineStr"/>
-      <c r="Q95" t="inlineStr"/>
-      <c r="R95" t="inlineStr">
-        <is>
-          <t>http://purl.org/np/RAjk9ru697It_UawXK1gvq-mpaOdGlwyhNb9nF2tfEE2A</t>
-        </is>
-      </c>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>https://orcid.org/0000-0003-2195-3997</t>
-        </is>
-      </c>
-      <c r="T95" t="inlineStr">
-        <is>
-          <t>2023-08-16</t>
-        </is>
-      </c>
-      <c r="U95" t="inlineStr">
-        <is>
-          <t>2023-08-23</t>
-        </is>
-      </c>
-      <c r="V95" t="inlineStr"/>
-      <c r="W95" t="inlineStr"/>
-      <c r="X95" t="inlineStr"/>
-      <c r="Y95" t="inlineStr"/>
-      <c r="Z95" t="inlineStr"/>
-      <c r="AA95" t="inlineStr"/>
-      <c r="AB95" t="inlineStr"/>
-      <c r="AC95" t="inlineStr"/>
-      <c r="AD95" t="inlineStr"/>
-      <c r="AE95" t="inlineStr"/>
-      <c r="AF95" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New SO vocabulary files generated (TTL, XLSX)
</commit_message>
<xml_diff>
--- a/standard-observations.xlsx
+++ b/standard-observations.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG107"/>
+  <dimension ref="A1:AF107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>https://vocabs.lter-europe.net/so/</t>
+          <t>http://vocabs.lter-europe.net/so/</t>
         </is>
       </c>
       <c r="C1" t="inlineStr"/>
@@ -462,7 +462,6 @@
       <c r="AD1" t="inlineStr"/>
       <c r="AE1" t="inlineStr"/>
       <c r="AF1" t="inlineStr"/>
-      <c r="AG1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -509,7 +508,6 @@
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -556,7 +554,6 @@
       <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -603,7 +600,6 @@
       <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -650,7 +646,6 @@
       <c r="AD5" t="inlineStr"/>
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -697,7 +692,6 @@
       <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -744,7 +738,6 @@
       <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -791,7 +784,6 @@
       <c r="AD8" t="inlineStr"/>
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -838,7 +830,6 @@
       <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -885,7 +876,6 @@
       <c r="AD10" t="inlineStr"/>
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -932,7 +922,6 @@
       <c r="AD11" t="inlineStr"/>
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr"/>
-      <c r="AG11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -979,7 +968,6 @@
       <c r="AD12" t="inlineStr"/>
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="inlineStr"/>
-      <c r="AG12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1026,7 +1014,6 @@
       <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1073,7 +1060,6 @@
       <c r="AD14" t="inlineStr"/>
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr"/>
-      <c r="AG14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1120,7 +1106,6 @@
       <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1167,7 +1152,6 @@
       <c r="AD16" t="inlineStr"/>
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1210,7 +1194,6 @@
       <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="inlineStr"/>
-      <c r="AG17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1253,7 +1236,6 @@
       <c r="AD18" t="inlineStr"/>
       <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="inlineStr"/>
-      <c r="AG18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1296,7 +1278,6 @@
       <c r="AD19" t="inlineStr"/>
       <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr"/>
-      <c r="AG19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1339,7 +1320,6 @@
       <c r="AD20" t="inlineStr"/>
       <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="inlineStr"/>
-      <c r="AG20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1382,7 +1362,6 @@
       <c r="AD21" t="inlineStr"/>
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr"/>
-      <c r="AG21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1425,7 +1404,6 @@
       <c r="AD22" t="inlineStr"/>
       <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="inlineStr"/>
-      <c r="AG22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1468,7 +1446,6 @@
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr"/>
       <c r="AF23" t="inlineStr"/>
-      <c r="AG23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1478,7 +1455,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>CC-BY 4.0</t>
+          <t>https://creativecommons.org/licenses/by/4.0/</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -1511,7 +1488,6 @@
       <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="inlineStr"/>
       <c r="AF24" t="inlineStr"/>
-      <c r="AG24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1521,7 +1497,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0.0.3</t>
+          <t>1.1.3</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -1554,7 +1530,6 @@
       <c r="AD25" t="inlineStr"/>
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr"/>
-      <c r="AG25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1564,7 +1539,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2023-08-16T11:00:00+00:00</t>
+          <t>2023-08-16</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -1597,7 +1572,6 @@
       <c r="AD26" t="inlineStr"/>
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr"/>
-      <c r="AG26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1607,7 +1581,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-06-13</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -1640,7 +1614,6 @@
       <c r="AD27" t="inlineStr"/>
       <c r="AE27" t="inlineStr"/>
       <c r="AF27" t="inlineStr"/>
-      <c r="AG27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1650,7 +1623,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://vocabs.lter-europe.net/so/</t>
+          <t>http://vocabs.lter-europe.net/so/</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -1683,7 +1656,6 @@
       <c r="AD28" t="inlineStr"/>
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr"/>
-      <c r="AG28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1726,7 +1698,6 @@
       <c r="AD29" t="inlineStr"/>
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr"/>
-      <c r="AG29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1769,7 +1740,6 @@
       <c r="AD30" t="inlineStr"/>
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr"/>
-      <c r="AG30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1812,7 +1782,6 @@
       <c r="AD31" t="inlineStr"/>
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr"/>
-      <c r="AG31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1855,7 +1824,6 @@
       <c r="AD32" t="inlineStr"/>
       <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr"/>
-      <c r="AG32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1898,7 +1866,6 @@
       <c r="AD33" t="inlineStr"/>
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" t="inlineStr"/>
-      <c r="AG33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1941,7 +1908,6 @@
       <c r="AD34" t="inlineStr"/>
       <c r="AE34" t="inlineStr"/>
       <c r="AF34" t="inlineStr"/>
-      <c r="AG34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1984,7 +1950,6 @@
       <c r="AD35" t="inlineStr"/>
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr"/>
-      <c r="AG35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2027,7 +1992,6 @@
       <c r="AD36" t="inlineStr"/>
       <c r="AE36" t="inlineStr"/>
       <c r="AF36" t="inlineStr"/>
-      <c r="AG36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2070,7 +2034,6 @@
       <c r="AD37" t="inlineStr"/>
       <c r="AE37" t="inlineStr"/>
       <c r="AF37" t="inlineStr"/>
-      <c r="AG37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2113,7 +2076,6 @@
       <c r="AD38" t="inlineStr"/>
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr"/>
-      <c r="AG38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2232,7 +2194,6 @@
       <c r="AD39" t="inlineStr"/>
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr"/>
-      <c r="AG39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2284,7 +2245,7 @@
       </c>
       <c r="T40" t="inlineStr">
         <is>
-          <t>2023-08-16</t>
+          <t>8/16/2023</t>
         </is>
       </c>
       <c r="U40" t="inlineStr">
@@ -2303,7 +2264,6 @@
       <c r="AD40" t="inlineStr"/>
       <c r="AE40" t="inlineStr"/>
       <c r="AF40" t="inlineStr"/>
-      <c r="AG40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2374,7 +2334,6 @@
       <c r="AD41" t="inlineStr"/>
       <c r="AE41" t="inlineStr"/>
       <c r="AF41" t="inlineStr"/>
-      <c r="AG41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2445,7 +2404,6 @@
       <c r="AD42" t="inlineStr"/>
       <c r="AE42" t="inlineStr"/>
       <c r="AF42" t="inlineStr"/>
-      <c r="AG42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2516,7 +2474,6 @@
       <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
       <c r="AF43" t="inlineStr"/>
-      <c r="AG43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2587,7 +2544,6 @@
       <c r="AD44" t="inlineStr"/>
       <c r="AE44" t="inlineStr"/>
       <c r="AF44" t="inlineStr"/>
-      <c r="AG44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2597,7 +2553,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CO2 flux and concentration, Latent heat flux, Sensible heat flux - Eddy Covariance</t>
+          <t>Eddy Covariance (CO2 flux and concentration, Latent heat flux, Sensible heat flux)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2644,7 +2600,7 @@
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>2023-08-23</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V45" t="inlineStr"/>
@@ -2658,7 +2614,6 @@
       <c r="AD45" t="inlineStr"/>
       <c r="AE45" t="inlineStr"/>
       <c r="AF45" t="inlineStr"/>
-      <c r="AG45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2729,7 +2684,6 @@
       <c r="AD46" t="inlineStr"/>
       <c r="AE46" t="inlineStr"/>
       <c r="AF46" t="inlineStr"/>
-      <c r="AG46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2739,7 +2693,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Vegetation phenology and Leaf Area Index – European scale</t>
+          <t>Vegetation phenology and Leaf Area Index - European scale</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2786,7 +2740,7 @@
       </c>
       <c r="U47" t="inlineStr">
         <is>
-          <t>2023-08-23</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V47" t="inlineStr"/>
@@ -2800,7 +2754,6 @@
       <c r="AD47" t="inlineStr"/>
       <c r="AE47" t="inlineStr"/>
       <c r="AF47" t="inlineStr"/>
-      <c r="AG47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2810,7 +2763,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Vegetation phenology – site scale</t>
+          <t>Vegetation phenology - site scale</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2857,7 +2810,7 @@
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>2023-08-23</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V48" t="inlineStr"/>
@@ -2871,7 +2824,6 @@
       <c r="AD48" t="inlineStr"/>
       <c r="AE48" t="inlineStr"/>
       <c r="AF48" t="inlineStr"/>
-      <c r="AG48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2942,7 +2894,6 @@
       <c r="AD49" t="inlineStr"/>
       <c r="AE49" t="inlineStr"/>
       <c r="AF49" t="inlineStr"/>
-      <c r="AG49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3013,7 +2964,6 @@
       <c r="AD50" t="inlineStr"/>
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr"/>
-      <c r="AG50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3084,7 +3034,6 @@
       <c r="AD51" t="inlineStr"/>
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" t="inlineStr"/>
-      <c r="AG51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3141,7 +3090,7 @@
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>2023-08-23</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="V52" t="inlineStr"/>
@@ -3155,7 +3104,6 @@
       <c r="AD52" t="inlineStr"/>
       <c r="AE52" t="inlineStr"/>
       <c r="AF52" t="inlineStr"/>
-      <c r="AG52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3212,7 +3160,7 @@
       </c>
       <c r="U53" t="inlineStr">
         <is>
-          <t>2023-08-23</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="V53" t="inlineStr"/>
@@ -3226,7 +3174,6 @@
       <c r="AD53" t="inlineStr"/>
       <c r="AE53" t="inlineStr"/>
       <c r="AF53" t="inlineStr"/>
-      <c r="AG53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3297,7 +3244,6 @@
       <c r="AD54" t="inlineStr"/>
       <c r="AE54" t="inlineStr"/>
       <c r="AF54" t="inlineStr"/>
-      <c r="AG54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3307,7 +3253,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Vegetation aboveground biomass – non-forested sites</t>
+          <t>Vegetation aboveground biomass - non-forested sites</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3354,7 +3300,7 @@
       </c>
       <c r="U55" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V55" t="inlineStr"/>
@@ -3368,7 +3314,6 @@
       <c r="AD55" t="inlineStr"/>
       <c r="AE55" t="inlineStr"/>
       <c r="AF55" t="inlineStr"/>
-      <c r="AG55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3439,7 +3384,6 @@
       <c r="AD56" t="inlineStr"/>
       <c r="AE56" t="inlineStr"/>
       <c r="AF56" t="inlineStr"/>
-      <c r="AG56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3449,7 +3393,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Leaf area index – non-forested sites</t>
+          <t>Leaf area index - non-forested sites</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3496,7 +3440,7 @@
       </c>
       <c r="U57" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V57" t="inlineStr"/>
@@ -3510,7 +3454,6 @@
       <c r="AD57" t="inlineStr"/>
       <c r="AE57" t="inlineStr"/>
       <c r="AF57" t="inlineStr"/>
-      <c r="AG57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3581,7 +3524,6 @@
       <c r="AD58" t="inlineStr"/>
       <c r="AE58" t="inlineStr"/>
       <c r="AF58" t="inlineStr"/>
-      <c r="AG58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3652,7 +3594,6 @@
       <c r="AD59" t="inlineStr"/>
       <c r="AE59" t="inlineStr"/>
       <c r="AF59" t="inlineStr"/>
-      <c r="AG59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3723,7 +3664,6 @@
       <c r="AD60" t="inlineStr"/>
       <c r="AE60" t="inlineStr"/>
       <c r="AF60" t="inlineStr"/>
-      <c r="AG60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3794,7 +3734,6 @@
       <c r="AD61" t="inlineStr"/>
       <c r="AE61" t="inlineStr"/>
       <c r="AF61" t="inlineStr"/>
-      <c r="AG61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3865,7 +3804,6 @@
       <c r="AD62" t="inlineStr"/>
       <c r="AE62" t="inlineStr"/>
       <c r="AF62" t="inlineStr"/>
-      <c r="AG62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3936,7 +3874,6 @@
       <c r="AD63" t="inlineStr"/>
       <c r="AE63" t="inlineStr"/>
       <c r="AF63" t="inlineStr"/>
-      <c r="AG63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4007,7 +3944,6 @@
       <c r="AD64" t="inlineStr"/>
       <c r="AE64" t="inlineStr"/>
       <c r="AF64" t="inlineStr"/>
-      <c r="AG64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4078,7 +4014,6 @@
       <c r="AD65" t="inlineStr"/>
       <c r="AE65" t="inlineStr"/>
       <c r="AF65" t="inlineStr"/>
-      <c r="AG65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4149,7 +4084,6 @@
       <c r="AD66" t="inlineStr"/>
       <c r="AE66" t="inlineStr"/>
       <c r="AF66" t="inlineStr"/>
-      <c r="AG66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4220,7 +4154,6 @@
       <c r="AD67" t="inlineStr"/>
       <c r="AE67" t="inlineStr"/>
       <c r="AF67" t="inlineStr"/>
-      <c r="AG67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4291,7 +4224,6 @@
       <c r="AD68" t="inlineStr"/>
       <c r="AE68" t="inlineStr"/>
       <c r="AF68" t="inlineStr"/>
-      <c r="AG68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -4362,7 +4294,6 @@
       <c r="AD69" t="inlineStr"/>
       <c r="AE69" t="inlineStr"/>
       <c r="AF69" t="inlineStr"/>
-      <c r="AG69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -4433,7 +4364,6 @@
       <c r="AD70" t="inlineStr"/>
       <c r="AE70" t="inlineStr"/>
       <c r="AF70" t="inlineStr"/>
-      <c r="AG70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -4504,7 +4434,6 @@
       <c r="AD71" t="inlineStr"/>
       <c r="AE71" t="inlineStr"/>
       <c r="AF71" t="inlineStr"/>
-      <c r="AG71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4575,7 +4504,6 @@
       <c r="AD72" t="inlineStr"/>
       <c r="AE72" t="inlineStr"/>
       <c r="AF72" t="inlineStr"/>
-      <c r="AG72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4646,7 +4574,6 @@
       <c r="AD73" t="inlineStr"/>
       <c r="AE73" t="inlineStr"/>
       <c r="AF73" t="inlineStr"/>
-      <c r="AG73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4717,7 +4644,6 @@
       <c r="AD74" t="inlineStr"/>
       <c r="AE74" t="inlineStr"/>
       <c r="AF74" t="inlineStr"/>
-      <c r="AG74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4788,7 +4714,6 @@
       <c r="AD75" t="inlineStr"/>
       <c r="AE75" t="inlineStr"/>
       <c r="AF75" t="inlineStr"/>
-      <c r="AG75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4859,7 +4784,6 @@
       <c r="AD76" t="inlineStr"/>
       <c r="AE76" t="inlineStr"/>
       <c r="AF76" t="inlineStr"/>
-      <c r="AG76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4869,7 +4793,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Major ion concentrations: Cl, SO4, Br, Na, K, Mg, Ca - groundwater</t>
+          <t>Major ion concentrations: Cl, SO4, Br, Na, K, Mg, Ca, B - groundwater</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -4916,7 +4840,7 @@
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V77" t="inlineStr"/>
@@ -4930,7 +4854,6 @@
       <c r="AD77" t="inlineStr"/>
       <c r="AE77" t="inlineStr"/>
       <c r="AF77" t="inlineStr"/>
-      <c r="AG77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -5001,7 +4924,6 @@
       <c r="AD78" t="inlineStr"/>
       <c r="AE78" t="inlineStr"/>
       <c r="AF78" t="inlineStr"/>
-      <c r="AG78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -5072,7 +4994,6 @@
       <c r="AD79" t="inlineStr"/>
       <c r="AE79" t="inlineStr"/>
       <c r="AF79" t="inlineStr"/>
-      <c r="AG79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -5143,7 +5064,6 @@
       <c r="AD80" t="inlineStr"/>
       <c r="AE80" t="inlineStr"/>
       <c r="AF80" t="inlineStr"/>
-      <c r="AG80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -5214,7 +5134,6 @@
       <c r="AD81" t="inlineStr"/>
       <c r="AE81" t="inlineStr"/>
       <c r="AF81" t="inlineStr"/>
-      <c r="AG81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -5285,7 +5204,6 @@
       <c r="AD82" t="inlineStr"/>
       <c r="AE82" t="inlineStr"/>
       <c r="AF82" t="inlineStr"/>
-      <c r="AG82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -5295,7 +5213,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Nutrient concentration: DOC, DIC - running waters</t>
+          <t>Carbon concentration: DOC, DIC - running waters</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -5342,7 +5260,7 @@
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V83" t="inlineStr"/>
@@ -5356,7 +5274,6 @@
       <c r="AD83" t="inlineStr"/>
       <c r="AE83" t="inlineStr"/>
       <c r="AF83" t="inlineStr"/>
-      <c r="AG83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -5427,7 +5344,6 @@
       <c r="AD84" t="inlineStr"/>
       <c r="AE84" t="inlineStr"/>
       <c r="AF84" t="inlineStr"/>
-      <c r="AG84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -5437,7 +5353,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Major ion concentrations: Cl, SO4, Br, Na, K, Mg, Ca, B, Silica - inland running/standing waters, transitional waters</t>
+          <t>Major ion concentrations: Cl, SO4, Br, Na, K, Mg, Ca, B, Silica - running/standing waters</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -5484,7 +5400,7 @@
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>2024-07-07</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V85" t="inlineStr"/>
@@ -5498,7 +5414,6 @@
       <c r="AD85" t="inlineStr"/>
       <c r="AE85" t="inlineStr"/>
       <c r="AF85" t="inlineStr"/>
-      <c r="AG85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -5569,7 +5484,6 @@
       <c r="AD86" t="inlineStr"/>
       <c r="AE86" t="inlineStr"/>
       <c r="AF86" t="inlineStr"/>
-      <c r="AG86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -5640,7 +5554,6 @@
       <c r="AD87" t="inlineStr"/>
       <c r="AE87" t="inlineStr"/>
       <c r="AF87" t="inlineStr"/>
-      <c r="AG87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -5711,7 +5624,6 @@
       <c r="AD88" t="inlineStr"/>
       <c r="AE88" t="inlineStr"/>
       <c r="AF88" t="inlineStr"/>
-      <c r="AG88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -5786,7 +5698,6 @@
       <c r="AD89" t="inlineStr"/>
       <c r="AE89" t="inlineStr"/>
       <c r="AF89" t="inlineStr"/>
-      <c r="AG89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -5853,7 +5764,6 @@
       <c r="AD90" t="inlineStr"/>
       <c r="AE90" t="inlineStr"/>
       <c r="AF90" t="inlineStr"/>
-      <c r="AG90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5920,7 +5830,6 @@
       <c r="AD91" t="inlineStr"/>
       <c r="AE91" t="inlineStr"/>
       <c r="AF91" t="inlineStr"/>
-      <c r="AG91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5987,7 +5896,6 @@
       <c r="AD92" t="inlineStr"/>
       <c r="AE92" t="inlineStr"/>
       <c r="AF92" t="inlineStr"/>
-      <c r="AG92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -6054,7 +5962,6 @@
       <c r="AD93" t="inlineStr"/>
       <c r="AE93" t="inlineStr"/>
       <c r="AF93" t="inlineStr"/>
-      <c r="AG93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -6121,7 +6028,6 @@
       <c r="AD94" t="inlineStr"/>
       <c r="AE94" t="inlineStr"/>
       <c r="AF94" t="inlineStr"/>
-      <c r="AG94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -6192,7 +6098,6 @@
       <c r="AD95" t="inlineStr"/>
       <c r="AE95" t="inlineStr"/>
       <c r="AF95" t="inlineStr"/>
-      <c r="AG95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -6263,7 +6168,6 @@
       <c r="AD96" t="inlineStr"/>
       <c r="AE96" t="inlineStr"/>
       <c r="AF96" t="inlineStr"/>
-      <c r="AG96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -6334,7 +6238,6 @@
       <c r="AD97" t="inlineStr"/>
       <c r="AE97" t="inlineStr"/>
       <c r="AF97" t="inlineStr"/>
-      <c r="AG97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -6405,7 +6308,6 @@
       <c r="AD98" t="inlineStr"/>
       <c r="AE98" t="inlineStr"/>
       <c r="AF98" t="inlineStr"/>
-      <c r="AG98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -6476,7 +6378,6 @@
       <c r="AD99" t="inlineStr"/>
       <c r="AE99" t="inlineStr"/>
       <c r="AF99" t="inlineStr"/>
-      <c r="AG99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -6486,7 +6387,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Land cover, land use (Statistics) and (for Platforms only) land use actors</t>
+          <t>Land cover, land use, land cover change, land use change (Statistics)</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -6533,7 +6434,7 @@
       </c>
       <c r="U100" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V100" t="inlineStr"/>
@@ -6547,7 +6448,6 @@
       <c r="AD100" t="inlineStr"/>
       <c r="AE100" t="inlineStr"/>
       <c r="AF100" t="inlineStr"/>
-      <c r="AG100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -6618,7 +6518,6 @@
       <c r="AD101" t="inlineStr"/>
       <c r="AE101" t="inlineStr"/>
       <c r="AF101" t="inlineStr"/>
-      <c r="AG101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -6689,7 +6588,6 @@
       <c r="AD102" t="inlineStr"/>
       <c r="AE102" t="inlineStr"/>
       <c r="AF102" t="inlineStr"/>
-      <c r="AG102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -6760,7 +6658,6 @@
       <c r="AD103" t="inlineStr"/>
       <c r="AE103" t="inlineStr"/>
       <c r="AF103" t="inlineStr"/>
-      <c r="AG103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -6831,7 +6728,6 @@
       <c r="AD104" t="inlineStr"/>
       <c r="AE104" t="inlineStr"/>
       <c r="AF104" t="inlineStr"/>
-      <c r="AG104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -6902,7 +6798,6 @@
       <c r="AD105" t="inlineStr"/>
       <c r="AE105" t="inlineStr"/>
       <c r="AF105" t="inlineStr"/>
-      <c r="AG105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -6912,7 +6807,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Resource use (MFA)</t>
+          <t>Resource use</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -6959,7 +6854,7 @@
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="V106" t="inlineStr"/>
@@ -6973,7 +6868,6 @@
       <c r="AD106" t="inlineStr"/>
       <c r="AE106" t="inlineStr"/>
       <c r="AF106" t="inlineStr"/>
-      <c r="AG106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -7044,7 +6938,6 @@
       <c r="AD107" t="inlineStr"/>
       <c r="AE107" t="inlineStr"/>
       <c r="AF107" t="inlineStr"/>
-      <c r="AG107" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>